<commit_message>
removed costaria with obvious length typo
</commit_message>
<xml_diff>
--- a/GW_kelp_phenology_data.xlsx
+++ b/GW_kelp_phenology_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sschenk_student_ubc_ca/Documents/Project - Seaweed Seasonality Transects/seaweed_seasonality_2021-09-05/git_GW_seaweed_seasonality_transects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="715" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2C8B2E7-3C64-4F20-8A02-AAB78F6539FC}"/>
+  <xr:revisionPtr revIDLastSave="718" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BAB354B-96FA-4C84-81E9-82537A1470AF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$90</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$121</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="20">
   <si>
     <t>year</t>
   </si>
@@ -470,11 +470,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L122"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:L121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E123" sqref="E123"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A83" sqref="A83:XFD83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,7 +528,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2024</v>
       </c>
@@ -556,7 +557,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -585,7 +586,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2024</v>
       </c>
@@ -614,7 +615,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2024</v>
       </c>
@@ -643,7 +644,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2024</v>
       </c>
@@ -672,7 +673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2024</v>
       </c>
@@ -701,7 +702,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -730,7 +731,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2024</v>
       </c>
@@ -759,7 +760,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2024</v>
       </c>
@@ -788,7 +789,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2024</v>
       </c>
@@ -817,7 +818,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2024</v>
       </c>
@@ -846,7 +847,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2024</v>
       </c>
@@ -875,7 +876,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2024</v>
       </c>
@@ -910,7 +911,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2024</v>
       </c>
@@ -945,7 +946,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2024</v>
       </c>
@@ -980,7 +981,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2024</v>
       </c>
@@ -1015,7 +1016,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2024</v>
       </c>
@@ -1050,7 +1051,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2024</v>
       </c>
@@ -1079,7 +1080,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2024</v>
       </c>
@@ -1108,7 +1109,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2024</v>
       </c>
@@ -1137,7 +1138,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2024</v>
       </c>
@@ -1166,7 +1167,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2024</v>
       </c>
@@ -1195,7 +1196,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2024</v>
       </c>
@@ -1224,7 +1225,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2024</v>
       </c>
@@ -1253,7 +1254,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2024</v>
       </c>
@@ -1282,7 +1283,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2024</v>
       </c>
@@ -1311,7 +1312,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2024</v>
       </c>
@@ -1340,7 +1341,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2024</v>
       </c>
@@ -1369,7 +1370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2024</v>
       </c>
@@ -1398,7 +1399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2024</v>
       </c>
@@ -1427,7 +1428,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2024</v>
       </c>
@@ -1456,7 +1457,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2024</v>
       </c>
@@ -1485,7 +1486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2024</v>
       </c>
@@ -1514,7 +1515,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2024</v>
       </c>
@@ -1543,7 +1544,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2024</v>
       </c>
@@ -1572,7 +1573,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2024</v>
       </c>
@@ -1601,7 +1602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2024</v>
       </c>
@@ -1630,7 +1631,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2024</v>
       </c>
@@ -1659,7 +1660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2024</v>
       </c>
@@ -1688,7 +1689,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2024</v>
       </c>
@@ -1717,7 +1718,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2024</v>
       </c>
@@ -1746,7 +1747,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2024</v>
       </c>
@@ -1781,7 +1782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2024</v>
       </c>
@@ -1813,7 +1814,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2024</v>
       </c>
@@ -1848,7 +1849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2024</v>
       </c>
@@ -1880,7 +1881,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2024</v>
       </c>
@@ -1915,7 +1916,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2024</v>
       </c>
@@ -1950,7 +1951,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2024</v>
       </c>
@@ -1982,7 +1983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2024</v>
       </c>
@@ -2017,7 +2018,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2024</v>
       </c>
@@ -2046,7 +2047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2024</v>
       </c>
@@ -2075,7 +2076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2024</v>
       </c>
@@ -2104,7 +2105,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2024</v>
       </c>
@@ -2133,7 +2134,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2024</v>
       </c>
@@ -2168,7 +2169,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2024</v>
       </c>
@@ -2200,7 +2201,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2024</v>
       </c>
@@ -2232,7 +2233,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2024</v>
       </c>
@@ -2264,7 +2265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2024</v>
       </c>
@@ -2296,7 +2297,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2024</v>
       </c>
@@ -2331,7 +2332,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2024</v>
       </c>
@@ -2366,7 +2367,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2024</v>
       </c>
@@ -2398,7 +2399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2024</v>
       </c>
@@ -2433,7 +2434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2024</v>
       </c>
@@ -2468,7 +2469,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2024</v>
       </c>
@@ -2497,7 +2498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2024</v>
       </c>
@@ -2526,7 +2527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2024</v>
       </c>
@@ -2555,7 +2556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2024</v>
       </c>
@@ -2584,7 +2585,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2024</v>
       </c>
@@ -2613,7 +2614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2024</v>
       </c>
@@ -2642,7 +2643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2024</v>
       </c>
@@ -2671,7 +2672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2024</v>
       </c>
@@ -2700,7 +2701,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2024</v>
       </c>
@@ -2729,7 +2730,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2024</v>
       </c>
@@ -2758,7 +2759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>2024</v>
       </c>
@@ -2787,7 +2788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2024</v>
       </c>
@@ -2822,7 +2823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2024</v>
       </c>
@@ -2851,7 +2852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>2024</v>
       </c>
@@ -2880,7 +2881,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2024</v>
       </c>
@@ -2909,7 +2910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2024</v>
       </c>
@@ -2938,7 +2939,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2024</v>
       </c>
@@ -2967,7 +2968,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>2024</v>
       </c>
@@ -3010,13 +3011,13 @@
         <v>7</v>
       </c>
       <c r="E83">
-        <v>11.5</v>
+        <v>86</v>
       </c>
       <c r="F83">
-        <v>29.5</v>
+        <v>25</v>
       </c>
       <c r="I83">
-        <v>121.5</v>
+        <v>55.4</v>
       </c>
       <c r="J83" t="s">
         <v>14</v>
@@ -3025,7 +3026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>2024</v>
       </c>
@@ -3036,16 +3037,13 @@
         <v>12</v>
       </c>
       <c r="D84" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E84">
-        <v>86</v>
+        <v>87.5</v>
       </c>
       <c r="F84">
-        <v>25</v>
-      </c>
-      <c r="I84">
-        <v>55.4</v>
+        <v>18.5</v>
       </c>
       <c r="J84" t="s">
         <v>14</v>
@@ -3053,8 +3051,11 @@
       <c r="K84" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L84" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>2024</v>
       </c>
@@ -3068,22 +3069,22 @@
         <v>6</v>
       </c>
       <c r="E85">
-        <v>87.5</v>
+        <v>88.5</v>
       </c>
       <c r="F85">
-        <v>18.5</v>
+        <v>23.5</v>
+      </c>
+      <c r="I85">
+        <v>73.7</v>
       </c>
       <c r="J85" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="K85" t="s">
         <v>9</v>
       </c>
-      <c r="L85" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>2024</v>
       </c>
@@ -3097,13 +3098,13 @@
         <v>6</v>
       </c>
       <c r="E86">
-        <v>88.5</v>
+        <v>90</v>
       </c>
       <c r="F86">
-        <v>23.5</v>
+        <v>24</v>
       </c>
       <c r="I86">
-        <v>73.7</v>
+        <v>58.1</v>
       </c>
       <c r="J86" t="s">
         <v>9</v>
@@ -3112,7 +3113,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>2024</v>
       </c>
@@ -3126,13 +3127,13 @@
         <v>6</v>
       </c>
       <c r="E87">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F87">
-        <v>24</v>
+        <v>20.5</v>
       </c>
       <c r="I87">
-        <v>58.1</v>
+        <v>51.6</v>
       </c>
       <c r="J87" t="s">
         <v>9</v>
@@ -3141,7 +3142,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>2024</v>
       </c>
@@ -3152,16 +3153,16 @@
         <v>12</v>
       </c>
       <c r="D88" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E88">
-        <v>83</v>
+        <v>132.5</v>
       </c>
       <c r="F88">
-        <v>20.5</v>
+        <v>15</v>
       </c>
       <c r="I88">
-        <v>51.6</v>
+        <v>25.1</v>
       </c>
       <c r="J88" t="s">
         <v>9</v>
@@ -3170,7 +3171,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2024</v>
       </c>
@@ -3184,13 +3185,13 @@
         <v>8</v>
       </c>
       <c r="E89">
-        <v>132.5</v>
+        <v>118.5</v>
       </c>
       <c r="F89">
-        <v>15</v>
+        <v>22.5</v>
       </c>
       <c r="I89">
-        <v>25.1</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="J89" t="s">
         <v>9</v>
@@ -3199,7 +3200,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>2024</v>
       </c>
@@ -3213,13 +3214,13 @@
         <v>8</v>
       </c>
       <c r="E90">
-        <v>118.5</v>
+        <v>124</v>
       </c>
       <c r="F90">
-        <v>22.5</v>
+        <v>14.5</v>
       </c>
       <c r="I90">
-        <v>39.299999999999997</v>
+        <v>25.5</v>
       </c>
       <c r="J90" t="s">
         <v>9</v>
@@ -3228,7 +3229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>2024</v>
       </c>
@@ -3239,411 +3240,417 @@
         <v>12</v>
       </c>
       <c r="D91" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91">
+        <v>63.5</v>
+      </c>
+      <c r="F91">
+        <v>19</v>
+      </c>
+      <c r="I91">
+        <v>28.5</v>
+      </c>
+      <c r="J91" t="s">
+        <v>9</v>
+      </c>
+      <c r="K91" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>2024</v>
+      </c>
+      <c r="B92">
+        <v>4</v>
+      </c>
+      <c r="C92">
+        <v>12</v>
+      </c>
+      <c r="D92" t="s">
+        <v>6</v>
+      </c>
+      <c r="E92">
+        <v>72</v>
+      </c>
+      <c r="F92">
+        <v>18.5</v>
+      </c>
+      <c r="I92">
+        <v>35.6</v>
+      </c>
+      <c r="J92" t="s">
+        <v>9</v>
+      </c>
+      <c r="K92" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>2024</v>
+      </c>
+      <c r="B93">
+        <v>4</v>
+      </c>
+      <c r="C93">
+        <v>12</v>
+      </c>
+      <c r="D93" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93">
+        <v>90</v>
+      </c>
+      <c r="F93">
+        <v>17</v>
+      </c>
+      <c r="I93">
+        <v>46.3</v>
+      </c>
+      <c r="J93" t="s">
+        <v>14</v>
+      </c>
+      <c r="K93" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>2024</v>
+      </c>
+      <c r="B94">
+        <v>4</v>
+      </c>
+      <c r="C94">
+        <v>12</v>
+      </c>
+      <c r="D94" t="s">
+        <v>10</v>
+      </c>
+      <c r="E94">
+        <v>198.5</v>
+      </c>
+      <c r="G94">
+        <v>65.5</v>
+      </c>
+      <c r="H94">
+        <v>4.2</v>
+      </c>
+      <c r="I94">
+        <v>194</v>
+      </c>
+      <c r="J94" t="s">
+        <v>9</v>
+      </c>
+      <c r="K94" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>2024</v>
+      </c>
+      <c r="B95">
+        <v>4</v>
+      </c>
+      <c r="C95">
+        <v>12</v>
+      </c>
+      <c r="D95" t="s">
         <v>8</v>
       </c>
-      <c r="E91">
-        <v>124</v>
-      </c>
-      <c r="F91">
-        <v>14.5</v>
-      </c>
-      <c r="I91">
-        <v>25.5</v>
-      </c>
-      <c r="J91" t="s">
-        <v>9</v>
-      </c>
-      <c r="K91" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A92">
-        <v>2024</v>
-      </c>
-      <c r="B92">
-        <v>4</v>
-      </c>
-      <c r="C92">
-        <v>12</v>
-      </c>
-      <c r="D92" t="s">
-        <v>6</v>
-      </c>
-      <c r="E92">
-        <v>63.5</v>
-      </c>
-      <c r="F92">
+      <c r="E95">
+        <v>148</v>
+      </c>
+      <c r="F95">
+        <v>19.5</v>
+      </c>
+      <c r="I95">
+        <v>46</v>
+      </c>
+      <c r="J95" t="s">
+        <v>9</v>
+      </c>
+      <c r="K95" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>2024</v>
+      </c>
+      <c r="B96">
+        <v>4</v>
+      </c>
+      <c r="C96">
+        <v>12</v>
+      </c>
+      <c r="D96" t="s">
+        <v>7</v>
+      </c>
+      <c r="E96">
+        <v>82.5</v>
+      </c>
+      <c r="F96">
+        <v>21</v>
+      </c>
+      <c r="J96" t="s">
+        <v>9</v>
+      </c>
+      <c r="K96" t="s">
+        <v>9</v>
+      </c>
+      <c r="L96" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>2024</v>
+      </c>
+      <c r="B97">
+        <v>4</v>
+      </c>
+      <c r="C97">
+        <v>12</v>
+      </c>
+      <c r="D97" t="s">
+        <v>6</v>
+      </c>
+      <c r="E97">
+        <v>91</v>
+      </c>
+      <c r="F97">
+        <v>25</v>
+      </c>
+      <c r="I97">
+        <v>82</v>
+      </c>
+      <c r="J97" t="s">
+        <v>9</v>
+      </c>
+      <c r="K97" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>2024</v>
+      </c>
+      <c r="B98">
+        <v>4</v>
+      </c>
+      <c r="C98">
+        <v>12</v>
+      </c>
+      <c r="D98" t="s">
+        <v>6</v>
+      </c>
+      <c r="E98">
+        <v>177</v>
+      </c>
+      <c r="F98">
+        <v>26</v>
+      </c>
+      <c r="J98" t="s">
+        <v>14</v>
+      </c>
+      <c r="K98" t="s">
+        <v>9</v>
+      </c>
+      <c r="L98" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>2024</v>
+      </c>
+      <c r="B99">
+        <v>4</v>
+      </c>
+      <c r="C99">
+        <v>12</v>
+      </c>
+      <c r="D99" t="s">
+        <v>8</v>
+      </c>
+      <c r="E99">
+        <v>105</v>
+      </c>
+      <c r="F99">
+        <v>19.5</v>
+      </c>
+      <c r="I99">
+        <v>28.7</v>
+      </c>
+      <c r="J99" t="s">
+        <v>9</v>
+      </c>
+      <c r="K99" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>2024</v>
+      </c>
+      <c r="B100">
+        <v>4</v>
+      </c>
+      <c r="C100">
+        <v>12</v>
+      </c>
+      <c r="D100" t="s">
+        <v>10</v>
+      </c>
+      <c r="E100">
+        <v>205</v>
+      </c>
+      <c r="G100">
+        <v>58</v>
+      </c>
+      <c r="H100">
+        <v>5</v>
+      </c>
+      <c r="I100">
+        <v>355.9</v>
+      </c>
+      <c r="J100" t="s">
+        <v>9</v>
+      </c>
+      <c r="K100" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>2024</v>
+      </c>
+      <c r="B101">
+        <v>4</v>
+      </c>
+      <c r="C101">
+        <v>12</v>
+      </c>
+      <c r="D101" t="s">
+        <v>8</v>
+      </c>
+      <c r="E101">
+        <v>143</v>
+      </c>
+      <c r="F101">
+        <v>24</v>
+      </c>
+      <c r="I101">
+        <v>53.5</v>
+      </c>
+      <c r="J101" t="s">
+        <v>9</v>
+      </c>
+      <c r="K101" t="s">
+        <v>9</v>
+      </c>
+      <c r="L101" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>2024</v>
+      </c>
+      <c r="B102">
+        <v>4</v>
+      </c>
+      <c r="C102">
+        <v>12</v>
+      </c>
+      <c r="D102" t="s">
+        <v>10</v>
+      </c>
+      <c r="E102">
+        <v>98.5</v>
+      </c>
+      <c r="G102">
+        <v>31</v>
+      </c>
+      <c r="H102">
+        <v>3.1</v>
+      </c>
+      <c r="J102" t="s">
+        <v>9</v>
+      </c>
+      <c r="K102" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>2024</v>
+      </c>
+      <c r="B103">
+        <v>4</v>
+      </c>
+      <c r="C103">
+        <v>12</v>
+      </c>
+      <c r="D103" t="s">
+        <v>8</v>
+      </c>
+      <c r="E103">
+        <v>163</v>
+      </c>
+      <c r="F103">
+        <v>30.5</v>
+      </c>
+      <c r="J103" t="s">
+        <v>9</v>
+      </c>
+      <c r="K103" t="s">
+        <v>9</v>
+      </c>
+      <c r="L103" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>2024</v>
+      </c>
+      <c r="B104">
+        <v>4</v>
+      </c>
+      <c r="C104">
+        <v>12</v>
+      </c>
+      <c r="D104" t="s">
+        <v>10</v>
+      </c>
+      <c r="E104">
+        <v>241.5</v>
+      </c>
+      <c r="F104" t="s">
         <v>19</v>
       </c>
-      <c r="I92">
-        <v>28.5</v>
-      </c>
-      <c r="J92" t="s">
-        <v>9</v>
-      </c>
-      <c r="K92" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A93">
-        <v>2024</v>
-      </c>
-      <c r="B93">
-        <v>4</v>
-      </c>
-      <c r="C93">
-        <v>12</v>
-      </c>
-      <c r="D93" t="s">
-        <v>6</v>
-      </c>
-      <c r="E93">
-        <v>72</v>
-      </c>
-      <c r="F93">
-        <v>18.5</v>
-      </c>
-      <c r="I93">
-        <v>35.6</v>
-      </c>
-      <c r="J93" t="s">
-        <v>9</v>
-      </c>
-      <c r="K93" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A94">
-        <v>2024</v>
-      </c>
-      <c r="B94">
-        <v>4</v>
-      </c>
-      <c r="C94">
-        <v>12</v>
-      </c>
-      <c r="D94" t="s">
-        <v>6</v>
-      </c>
-      <c r="E94">
-        <v>90</v>
-      </c>
-      <c r="F94">
-        <v>17</v>
-      </c>
-      <c r="I94">
-        <v>46.3</v>
-      </c>
-      <c r="J94" t="s">
+      <c r="G104">
+        <v>99.5</v>
+      </c>
+      <c r="H104">
+        <v>3.8</v>
+      </c>
+      <c r="I104">
+        <v>221.5</v>
+      </c>
+      <c r="J104" t="s">
         <v>14</v>
       </c>
-      <c r="K94" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A95">
-        <v>2024</v>
-      </c>
-      <c r="B95">
-        <v>4</v>
-      </c>
-      <c r="C95">
-        <v>12</v>
-      </c>
-      <c r="D95" t="s">
-        <v>10</v>
-      </c>
-      <c r="E95">
-        <v>198.5</v>
-      </c>
-      <c r="G95">
-        <v>65.5</v>
-      </c>
-      <c r="H95">
-        <v>4.2</v>
-      </c>
-      <c r="I95">
-        <v>194</v>
-      </c>
-      <c r="J95" t="s">
-        <v>9</v>
-      </c>
-      <c r="K95" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A96">
-        <v>2024</v>
-      </c>
-      <c r="B96">
-        <v>4</v>
-      </c>
-      <c r="C96">
-        <v>12</v>
-      </c>
-      <c r="D96" t="s">
-        <v>8</v>
-      </c>
-      <c r="E96">
-        <v>148</v>
-      </c>
-      <c r="F96">
-        <v>19.5</v>
-      </c>
-      <c r="I96">
-        <v>46</v>
-      </c>
-      <c r="J96" t="s">
-        <v>9</v>
-      </c>
-      <c r="K96" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A97">
-        <v>2024</v>
-      </c>
-      <c r="B97">
-        <v>4</v>
-      </c>
-      <c r="C97">
-        <v>12</v>
-      </c>
-      <c r="D97" t="s">
-        <v>7</v>
-      </c>
-      <c r="E97">
-        <v>82.5</v>
-      </c>
-      <c r="F97">
-        <v>21</v>
-      </c>
-      <c r="J97" t="s">
-        <v>9</v>
-      </c>
-      <c r="K97" t="s">
-        <v>9</v>
-      </c>
-      <c r="L97" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A98">
-        <v>2024</v>
-      </c>
-      <c r="B98">
-        <v>4</v>
-      </c>
-      <c r="C98">
-        <v>12</v>
-      </c>
-      <c r="D98" t="s">
-        <v>6</v>
-      </c>
-      <c r="E98">
-        <v>91</v>
-      </c>
-      <c r="F98">
-        <v>25</v>
-      </c>
-      <c r="I98">
-        <v>82</v>
-      </c>
-      <c r="J98" t="s">
-        <v>9</v>
-      </c>
-      <c r="K98" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A99">
-        <v>2024</v>
-      </c>
-      <c r="B99">
-        <v>4</v>
-      </c>
-      <c r="C99">
-        <v>12</v>
-      </c>
-      <c r="D99" t="s">
-        <v>6</v>
-      </c>
-      <c r="E99">
-        <v>177</v>
-      </c>
-      <c r="F99">
-        <v>26</v>
-      </c>
-      <c r="J99" t="s">
-        <v>14</v>
-      </c>
-      <c r="K99" t="s">
-        <v>9</v>
-      </c>
-      <c r="L99" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A100">
-        <v>2024</v>
-      </c>
-      <c r="B100">
-        <v>4</v>
-      </c>
-      <c r="C100">
-        <v>12</v>
-      </c>
-      <c r="D100" t="s">
-        <v>8</v>
-      </c>
-      <c r="E100">
-        <v>105</v>
-      </c>
-      <c r="F100">
-        <v>19.5</v>
-      </c>
-      <c r="I100">
-        <v>28.7</v>
-      </c>
-      <c r="J100" t="s">
-        <v>9</v>
-      </c>
-      <c r="K100" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A101">
-        <v>2024</v>
-      </c>
-      <c r="B101">
-        <v>4</v>
-      </c>
-      <c r="C101">
-        <v>12</v>
-      </c>
-      <c r="D101" t="s">
-        <v>10</v>
-      </c>
-      <c r="E101">
-        <v>205</v>
-      </c>
-      <c r="G101">
-        <v>58</v>
-      </c>
-      <c r="H101">
-        <v>5</v>
-      </c>
-      <c r="I101">
-        <v>355.9</v>
-      </c>
-      <c r="J101" t="s">
-        <v>9</v>
-      </c>
-      <c r="K101" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A102">
-        <v>2024</v>
-      </c>
-      <c r="B102">
-        <v>4</v>
-      </c>
-      <c r="C102">
-        <v>12</v>
-      </c>
-      <c r="D102" t="s">
-        <v>8</v>
-      </c>
-      <c r="E102">
-        <v>143</v>
-      </c>
-      <c r="F102">
-        <v>24</v>
-      </c>
-      <c r="I102">
-        <v>53.5</v>
-      </c>
-      <c r="J102" t="s">
-        <v>9</v>
-      </c>
-      <c r="K102" t="s">
-        <v>9</v>
-      </c>
-      <c r="L102" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A103">
-        <v>2024</v>
-      </c>
-      <c r="B103">
-        <v>4</v>
-      </c>
-      <c r="C103">
-        <v>12</v>
-      </c>
-      <c r="D103" t="s">
-        <v>10</v>
-      </c>
-      <c r="E103">
-        <v>98.5</v>
-      </c>
-      <c r="G103">
-        <v>31</v>
-      </c>
-      <c r="H103">
-        <v>3.1</v>
-      </c>
-      <c r="J103" t="s">
-        <v>9</v>
-      </c>
-      <c r="K103" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A104">
-        <v>2024</v>
-      </c>
-      <c r="B104">
-        <v>4</v>
-      </c>
-      <c r="C104">
-        <v>12</v>
-      </c>
-      <c r="D104" t="s">
-        <v>8</v>
-      </c>
-      <c r="E104">
-        <v>163</v>
-      </c>
-      <c r="F104">
-        <v>30.5</v>
-      </c>
-      <c r="J104" t="s">
-        <v>9</v>
-      </c>
       <c r="K104" t="s">
         <v>9</v>
       </c>
-      <c r="L104" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>2024</v>
       </c>
@@ -3657,19 +3664,16 @@
         <v>10</v>
       </c>
       <c r="E105">
-        <v>241.5</v>
-      </c>
-      <c r="F105" t="s">
-        <v>19</v>
+        <v>211</v>
       </c>
       <c r="G105">
-        <v>99.5</v>
+        <v>55</v>
       </c>
       <c r="H105">
-        <v>3.8</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I105">
-        <v>221.5</v>
+        <v>326.89999999999998</v>
       </c>
       <c r="J105" t="s">
         <v>14</v>
@@ -3678,7 +3682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>2024</v>
       </c>
@@ -3692,16 +3696,16 @@
         <v>10</v>
       </c>
       <c r="E106">
-        <v>211</v>
+        <v>214.5</v>
       </c>
       <c r="G106">
-        <v>55</v>
+        <v>63.5</v>
       </c>
       <c r="H106">
         <v>4.5999999999999996</v>
       </c>
       <c r="I106">
-        <v>326.89999999999998</v>
+        <v>248.2</v>
       </c>
       <c r="J106" t="s">
         <v>14</v>
@@ -3710,7 +3714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>2024</v>
       </c>
@@ -3724,25 +3728,25 @@
         <v>10</v>
       </c>
       <c r="E107">
-        <v>214.5</v>
+        <v>146</v>
       </c>
       <c r="G107">
-        <v>63.5</v>
+        <v>39.5</v>
       </c>
       <c r="H107">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="I107">
-        <v>248.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="J107" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="K107" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L107" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>2024</v>
       </c>
@@ -3756,13 +3760,16 @@
         <v>10</v>
       </c>
       <c r="E108">
-        <v>146</v>
+        <v>194.5</v>
       </c>
       <c r="G108">
-        <v>39.5</v>
+        <v>55.5</v>
       </c>
       <c r="H108">
-        <v>4.0999999999999996</v>
+        <v>4.3</v>
+      </c>
+      <c r="I108">
+        <v>240.8</v>
       </c>
       <c r="J108" t="s">
         <v>9</v>
@@ -3770,11 +3777,8 @@
       <c r="K108" t="s">
         <v>9</v>
       </c>
-      <c r="L108" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>2024</v>
       </c>
@@ -3788,16 +3792,16 @@
         <v>10</v>
       </c>
       <c r="E109">
-        <v>194.5</v>
+        <v>177.5</v>
       </c>
       <c r="G109">
-        <v>55.5</v>
+        <v>49</v>
       </c>
       <c r="H109">
-        <v>4.3</v>
+        <v>4</v>
       </c>
       <c r="I109">
-        <v>240.8</v>
+        <v>162.5</v>
       </c>
       <c r="J109" t="s">
         <v>9</v>
@@ -3806,7 +3810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>2024</v>
       </c>
@@ -3820,16 +3824,16 @@
         <v>10</v>
       </c>
       <c r="E110">
-        <v>177.5</v>
+        <v>132</v>
       </c>
       <c r="G110">
-        <v>49</v>
+        <v>43.5</v>
       </c>
       <c r="H110">
-        <v>4</v>
+        <v>2.8</v>
       </c>
       <c r="I110">
-        <v>162.5</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="J110" t="s">
         <v>9</v>
@@ -3838,7 +3842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>2024</v>
       </c>
@@ -3849,19 +3853,16 @@
         <v>12</v>
       </c>
       <c r="D111" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E111">
-        <v>132</v>
-      </c>
-      <c r="G111">
-        <v>43.5</v>
-      </c>
-      <c r="H111">
-        <v>2.8</v>
+        <v>106</v>
+      </c>
+      <c r="F111">
+        <v>31</v>
       </c>
       <c r="I111">
-        <v>81.599999999999994</v>
+        <v>96.4</v>
       </c>
       <c r="J111" t="s">
         <v>9</v>
@@ -3870,7 +3871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>2024</v>
       </c>
@@ -3881,16 +3882,16 @@
         <v>12</v>
       </c>
       <c r="D112" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E112">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F112">
-        <v>31</v>
+        <v>20.5</v>
       </c>
       <c r="I112">
-        <v>96.4</v>
+        <v>67.3</v>
       </c>
       <c r="J112" t="s">
         <v>9</v>
@@ -3899,7 +3900,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>2024</v>
       </c>
@@ -3913,13 +3914,10 @@
         <v>6</v>
       </c>
       <c r="E113">
-        <v>101</v>
+        <v>114.5</v>
       </c>
       <c r="F113">
-        <v>20.5</v>
-      </c>
-      <c r="I113">
-        <v>67.3</v>
+        <v>24</v>
       </c>
       <c r="J113" t="s">
         <v>9</v>
@@ -3939,22 +3937,25 @@
         <v>12</v>
       </c>
       <c r="D114" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E114">
-        <v>114.5</v>
+        <v>117</v>
       </c>
       <c r="F114">
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="I114">
+        <v>109.7</v>
       </c>
       <c r="J114" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="K114" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>2024</v>
       </c>
@@ -3965,25 +3966,28 @@
         <v>12</v>
       </c>
       <c r="D115" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E115">
-        <v>117</v>
-      </c>
-      <c r="F115">
-        <v>30</v>
-      </c>
-      <c r="I115">
-        <v>109.7</v>
+        <v>178.5</v>
+      </c>
+      <c r="G115">
+        <v>49.5</v>
+      </c>
+      <c r="H115">
+        <v>4.0999999999999996</v>
       </c>
       <c r="J115" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="K115" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L115" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>2024</v>
       </c>
@@ -3997,13 +4001,13 @@
         <v>10</v>
       </c>
       <c r="E116">
-        <v>178.5</v>
+        <v>158</v>
       </c>
       <c r="G116">
-        <v>49.5</v>
+        <v>36</v>
       </c>
       <c r="H116">
-        <v>4.0999999999999996</v>
+        <v>4.3</v>
       </c>
       <c r="J116" t="s">
         <v>9</v>
@@ -4015,7 +4019,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>2024</v>
       </c>
@@ -4026,16 +4030,16 @@
         <v>12</v>
       </c>
       <c r="D117" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E117">
-        <v>158</v>
-      </c>
-      <c r="G117">
-        <v>36</v>
-      </c>
-      <c r="H117">
-        <v>4.3</v>
+        <v>122.5</v>
+      </c>
+      <c r="F117">
+        <v>23</v>
+      </c>
+      <c r="I117">
+        <v>45.4</v>
       </c>
       <c r="J117" t="s">
         <v>9</v>
@@ -4043,11 +4047,8 @@
       <c r="K117" t="s">
         <v>9</v>
       </c>
-      <c r="L117" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>2024</v>
       </c>
@@ -4058,45 +4059,45 @@
         <v>12</v>
       </c>
       <c r="D118" t="s">
+        <v>6</v>
+      </c>
+      <c r="E118">
+        <v>120</v>
+      </c>
+      <c r="F118">
+        <v>22</v>
+      </c>
+      <c r="I118">
+        <v>91.9</v>
+      </c>
+      <c r="J118" t="s">
+        <v>9</v>
+      </c>
+      <c r="K118" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>2024</v>
+      </c>
+      <c r="B119">
+        <v>4</v>
+      </c>
+      <c r="C119">
+        <v>12</v>
+      </c>
+      <c r="D119" t="s">
         <v>8</v>
       </c>
-      <c r="E118">
-        <v>122.5</v>
-      </c>
-      <c r="F118">
-        <v>23</v>
-      </c>
-      <c r="I118">
-        <v>45.4</v>
-      </c>
-      <c r="J118" t="s">
-        <v>9</v>
-      </c>
-      <c r="K118" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A119">
-        <v>2024</v>
-      </c>
-      <c r="B119">
-        <v>4</v>
-      </c>
-      <c r="C119">
-        <v>12</v>
-      </c>
-      <c r="D119" t="s">
-        <v>6</v>
-      </c>
       <c r="E119">
-        <v>120</v>
+        <v>164.5</v>
       </c>
       <c r="F119">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="I119">
-        <v>91.9</v>
+        <v>74</v>
       </c>
       <c r="J119" t="s">
         <v>9</v>
@@ -4105,7 +4106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>2024</v>
       </c>
@@ -4119,13 +4120,13 @@
         <v>8</v>
       </c>
       <c r="E120">
-        <v>164.5</v>
+        <v>144</v>
       </c>
       <c r="F120">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="I120">
-        <v>74</v>
+        <v>43.1</v>
       </c>
       <c r="J120" t="s">
         <v>9</v>
@@ -4134,7 +4135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>2024</v>
       </c>
@@ -4145,16 +4146,13 @@
         <v>12</v>
       </c>
       <c r="D121" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E121">
-        <v>144</v>
+        <v>99.5</v>
       </c>
       <c r="F121">
-        <v>21</v>
-      </c>
-      <c r="I121">
-        <v>43.1</v>
+        <v>36</v>
       </c>
       <c r="J121" t="s">
         <v>9</v>
@@ -4162,38 +4160,23 @@
       <c r="K121" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A122">
-        <v>2024</v>
-      </c>
-      <c r="B122">
-        <v>4</v>
-      </c>
-      <c r="C122">
-        <v>12</v>
-      </c>
-      <c r="D122" t="s">
-        <v>7</v>
-      </c>
-      <c r="E122">
-        <v>99.5</v>
-      </c>
-      <c r="F122">
-        <v>36</v>
-      </c>
-      <c r="J122" t="s">
-        <v>9</v>
-      </c>
-      <c r="K122" t="s">
-        <v>9</v>
-      </c>
-      <c r="L122" t="s">
+      <c r="L121" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L90" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L121" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="costaria"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="9">
+      <filters>
+        <filter val="yes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:C1" xr:uid="{46EA6B54-3D38-4F49-A94E-5B77B5CC845D}"/>
   </dataValidations>

</xml_diff>